<commit_message>
Added module 9 - PWM
</commit_message>
<xml_diff>
--- a/presencas.xlsx
+++ b/presencas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RGoncalves\Documents\GitHub\uControllers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F83EDFA-5B4A-4180-9B76-BD9E415AD0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34679FBC-04E0-4443-9824-DFF069C91BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{2C134D35-A1A9-423E-A6D5-46E3626C9871}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C134D35-A1A9-423E-A6D5-46E3626C9871}"/>
   </bookViews>
   <sheets>
     <sheet name="Presenças " sheetId="2" r:id="rId1"/>
@@ -166,8 +166,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -195,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -207,6 +215,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -242,7 +251,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34EAA067-62F6-4B4C-B513-756D53A25755}" name="Tabela13" displayName="Tabela13" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{415105AD-E60A-4B9F-BC5A-CBCCA20040E2}"/>
+  <autoFilter ref="A1:H29" xr:uid="{415105AD-E60A-4B9F-BC5A-CBCCA20040E2}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="2B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{5107CD91-FBBF-4B36-B6C2-880DD5B823D4}" name="N.º mecanográfico" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{8B829CA4-2422-42E8-B6DA-D4A61BD1091C}" name="Nome"/>
@@ -259,7 +274,13 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{415105AD-E60A-4B9F-BC5A-CBCCA20040E2}" name="Tabela1" displayName="Tabela1" ref="A1:E29" totalsRowShown="0">
-  <autoFilter ref="A1:E29" xr:uid="{415105AD-E60A-4B9F-BC5A-CBCCA20040E2}"/>
+  <autoFilter ref="A1:E29" xr:uid="{415105AD-E60A-4B9F-BC5A-CBCCA20040E2}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="2B"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBC31C63-AAC5-486D-81FB-6B360D950D22}" name="N.º mecanográfico" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{D308D6D6-4DA7-457C-9BEE-4A454DF09047}" name="Nome"/>
@@ -568,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD02E65E-F242-4BA5-8F7B-DDE81EEE038F}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -609,7 +630,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1181754</v>
       </c>
@@ -630,8 +651,14 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1190924</v>
       </c>
@@ -642,7 +669,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1200714</v>
       </c>
@@ -663,6 +690,12 @@
       <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
@@ -674,6 +707,12 @@
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -685,8 +724,14 @@
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1200968</v>
       </c>
@@ -697,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1200969</v>
       </c>
@@ -708,7 +753,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1201005</v>
       </c>
@@ -719,7 +764,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1201050</v>
       </c>
@@ -730,7 +775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1201128</v>
       </c>
@@ -741,7 +786,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1201132</v>
       </c>
@@ -752,7 +797,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1201150</v>
       </c>
@@ -773,8 +818,14 @@
       <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1201171</v>
       </c>
@@ -784,8 +835,14 @@
       <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1201223</v>
       </c>
@@ -795,8 +852,14 @@
       <c r="C18" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1201233</v>
       </c>
@@ -806,8 +869,14 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1201360</v>
       </c>
@@ -817,8 +886,14 @@
       <c r="C20" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1201362</v>
       </c>
@@ -829,7 +904,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1201370</v>
       </c>
@@ -839,8 +914,14 @@
       <c r="C22" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1201373</v>
       </c>
@@ -851,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1201441</v>
       </c>
@@ -862,7 +943,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1201482</v>
       </c>
@@ -873,7 +954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1201576</v>
       </c>
@@ -883,8 +964,14 @@
       <c r="C26" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D26" s="1">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1201672</v>
       </c>
@@ -894,8 +981,14 @@
       <c r="C27" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1201674</v>
       </c>
@@ -905,8 +998,14 @@
       <c r="C28" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1201675</v>
       </c>
@@ -916,6 +1015,15 @@
       <c r="C29" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -930,8 +1038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247E9641-19D1-4D0A-B592-557747540A4A}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -959,7 +1067,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1181754</v>
       </c>
@@ -987,7 +1095,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>1190924</v>
       </c>
@@ -998,7 +1106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1200714</v>
       </c>
@@ -1057,7 +1165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>1200968</v>
       </c>
@@ -1068,7 +1176,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>1200969</v>
       </c>
@@ -1079,7 +1187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>1201005</v>
       </c>
@@ -1090,7 +1198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1201050</v>
       </c>
@@ -1101,7 +1209,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>1201128</v>
       </c>
@@ -1112,7 +1220,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>1201132</v>
       </c>
@@ -1123,7 +1231,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1201150</v>
       </c>
@@ -1216,7 +1324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1201362</v>
       </c>
@@ -1241,7 +1349,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1201373</v>
       </c>
@@ -1252,7 +1360,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1201441</v>
       </c>
@@ -1263,7 +1371,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1201482</v>
       </c>

</xml_diff>

<commit_message>
projetos e material atualizados
</commit_message>
<xml_diff>
--- a/presencas.xlsx
+++ b/presencas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RGoncalves\Documents\GitHub\uControllers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5FA43B-2E96-41E0-9A24-CDA7EFB0DFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD53B8E-DD8F-43CA-8702-B69AE63B8B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C134D35-A1A9-423E-A6D5-46E3626C9871}"/>
   </bookViews>
@@ -638,7 +638,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Relatorios adicionados e avaliacao 2B feita
</commit_message>
<xml_diff>
--- a/presencas.xlsx
+++ b/presencas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RGoncalves\Documents\GitHub\uControllers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF472609-F73A-436B-9D3D-7A670F096269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCEFB88-2D77-43CA-ACEC-4AC570C006EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1440" yWindow="1440" windowWidth="14400" windowHeight="7270" xr2:uid="{2C134D35-A1A9-423E-A6D5-46E3626C9871}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2C134D35-A1A9-423E-A6D5-46E3626C9871}"/>
   </bookViews>
   <sheets>
     <sheet name="Presenças " sheetId="2" r:id="rId1"/>
@@ -638,7 +638,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -723,6 +723,15 @@
       <c r="F3">
         <v>1</v>
       </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -769,6 +778,15 @@
       <c r="F6">
         <v>1</v>
       </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
@@ -789,6 +807,15 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -809,6 +836,15 @@
       <c r="F8">
         <v>1</v>
       </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -920,8 +956,17 @@
       <c r="F16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>1201171</v>
       </c>
@@ -940,8 +985,17 @@
       <c r="F17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>1201223</v>
       </c>
@@ -960,8 +1014,17 @@
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>1201233</v>
       </c>
@@ -980,8 +1043,17 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>1201360</v>
       </c>
@@ -1000,8 +1072,17 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>1201362</v>
       </c>
@@ -1014,7 +1095,7 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>1201370</v>
       </c>
@@ -1033,8 +1114,17 @@
       <c r="F22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>1201373</v>
       </c>
@@ -1047,7 +1137,7 @@
       </c>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>1201441</v>
       </c>
@@ -1060,7 +1150,7 @@
       </c>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>1201482</v>
       </c>
@@ -1073,7 +1163,7 @@
       </c>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>1201576</v>
       </c>
@@ -1092,8 +1182,17 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>1201672</v>
       </c>
@@ -1112,8 +1211,17 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>1201674</v>
       </c>
@@ -1132,8 +1240,17 @@
       <c r="F28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>1201675</v>
       </c>
@@ -1152,8 +1269,17 @@
       <c r="F29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>1201361</v>
       </c>
@@ -1164,6 +1290,12 @@
         <v>48</v>
       </c>
       <c r="E30" s="5"/>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>